<commit_message>
Updated test and jenkinsfile
</commit_message>
<xml_diff>
--- a/cypress/fixtures/messageData.xlsx
+++ b/cypress/fixtures/messageData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Surprise Ngoveni\Documents\Projects\RestfulBookerPlatformTesting\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8BDE487-F932-484D-9848-FD1AF7135A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48C1140-84D9-438A-A3C7-07A11CDA032B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="47">
   <si>
     <t>title</t>
   </si>
@@ -148,16 +148,19 @@
     <t>Subject must be between 5 and 100 characters.</t>
   </si>
   <si>
-    <t>Testing api with a subject that has 12 characters</t>
-  </si>
-  <si>
-    <t>Test subject</t>
-  </si>
-  <si>
     <t>+2894568735456</t>
   </si>
   <si>
     <t>tadda@gmail.com</t>
+  </si>
+  <si>
+    <t>Subject must be between 5 and 100 characters</t>
+  </si>
+  <si>
+    <t>Testing api with a subject that has more than 100 characters</t>
+  </si>
+  <si>
+    <t>Testing the api with a very long subject written in the text box field to see if it can fit more that 30 characters</t>
   </si>
 </sst>
 </file>
@@ -557,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -812,7 +815,7 @@
         <v>29</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E10" t="s">
         <v>40</v>
@@ -829,19 +832,25 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
         <v>32</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" t="s">
         <v>44</v>
-      </c>
-      <c r="E11" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>